<commit_message>
Add Multiple Emloyees from Excel File HW
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/batch12excel.xlsx
+++ b/src/test/resources/testdata/batch12excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quytr\IdeaProjects\CucumberFrameworkBatch12\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quytr\IdeaProjects\TestNGFramework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0A8809-C0E1-41EB-80C2-9818661D0F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A451DE2-F92C-4FCF-9091-5BFB296BC692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1935" windowWidth="18960" windowHeight="13020" xr2:uid="{6F8F12F9-0F58-41A1-B0C5-C42D0B39478B}"/>
+    <workbookView xWindow="-18675" yWindow="1620" windowWidth="18195" windowHeight="7815" xr2:uid="{6F8F12F9-0F58-41A1-B0C5-C42D0B39478B}"/>
   </bookViews>
   <sheets>
     <sheet name="EmployeeData" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>FirstName</t>
   </si>
@@ -52,43 +52,49 @@
     <t>Password</t>
   </si>
   <si>
-    <t>MS</t>
-  </si>
-  <si>
     <t>Hum@nhrm123</t>
   </si>
   <si>
-    <t>Dell</t>
-  </si>
-  <si>
-    <t>Sasir</t>
-  </si>
-  <si>
-    <t>Lee</t>
-  </si>
-  <si>
     <t>C:\Users\quytr\Desktop\Batch12\imagebatch12.jpg</t>
   </si>
   <si>
     <t>Username</t>
   </si>
   <si>
-    <t>Adeyy</t>
-  </si>
-  <si>
-    <t>Poef</t>
-  </si>
-  <si>
-    <t>Lofd</t>
-  </si>
-  <si>
-    <t>crewr354</t>
-  </si>
-  <si>
-    <t>ftry3</t>
-  </si>
-  <si>
-    <t>suhn35</t>
+    <t>Jr</t>
+  </si>
+  <si>
+    <t>Chan</t>
+  </si>
+  <si>
+    <t>Jackie</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>Holland</t>
+  </si>
+  <si>
+    <t>Star</t>
+  </si>
+  <si>
+    <t>Lord</t>
+  </si>
+  <si>
+    <t>Cool</t>
+  </si>
+  <si>
+    <t>tom123ho</t>
+  </si>
+  <si>
+    <t>jack8943ch</t>
+  </si>
+  <si>
+    <t>star130lord</t>
+  </si>
+  <si>
+    <t>Sr</t>
   </si>
 </sst>
 </file>
@@ -454,7 +460,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,7 +487,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -489,62 +495,62 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
         <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>